<commit_message>
added notes and other images
</commit_message>
<xml_diff>
--- a/7thJune_2023/TestCaseDocument.xlsx
+++ b/7thJune_2023/TestCaseDocument.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarth\Desktop\SOFTWARE TESTING\May_2023_WeekDay_Batch\MANUAL_TESTING\7thJune_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5E46E3-2EB0-4F6C-A5EB-BDB3AA52E6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03503226-C8C0-4DE7-BF88-D30818F4E35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{27A98898-CDB7-4D16-8468-A0A79BA7F42D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{27A98898-CDB7-4D16-8468-A0A79BA7F42D}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="2" r:id="rId1"/>
-    <sheet name="Login" sheetId="1" r:id="rId2"/>
-    <sheet name="Register" sheetId="3" r:id="rId3"/>
-    <sheet name="Search" sheetId="4" r:id="rId4"/>
+    <sheet name="RTM" sheetId="5" r:id="rId2"/>
+    <sheet name="Login" sheetId="1" r:id="rId3"/>
+    <sheet name="Register" sheetId="3" r:id="rId4"/>
+    <sheet name="Search" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -152,12 +153,63 @@
   <si>
     <t>Serch</t>
   </si>
+  <si>
+    <t>TC_LF_002</t>
+  </si>
+  <si>
+    <t>Verifying logging into the application using valid email and invalid password</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' link
+2. Click on 'Login' option
+3. Enter valid email in the E-mail Address field
+4. Enter invalid password in the Password Field
+5. Click on Login button</t>
+  </si>
+  <si>
+    <t>Email - seleniumpanda@gmail.com
+Password - Selenium@123456</t>
+  </si>
+  <si>
+    <t>1. User navigates to login page
+2. System does not allow login with a warning message "Warning: No match for E-Mail Address and/or Password."</t>
+  </si>
+  <si>
+    <t>Req No</t>
+  </si>
+  <si>
+    <t>Req Desc</t>
+  </si>
+  <si>
+    <t>TestCase ID</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Req_1</t>
+  </si>
+  <si>
+    <t>Login to the application</t>
+  </si>
+  <si>
+    <t>TC_LF_001, TC_LF_002</t>
+  </si>
+  <si>
+    <t>TC_LF_001 - Pass, TC_LF_002 - Pass</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +227,22 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,6 +278,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,11 +717,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196A9B89-498A-482D-AE57-EC4824350B17}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="32.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="21.6640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368EC599-9F70-4A5B-B239-50909E85D68C}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.88671875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -719,6 +840,41 @@
       <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -726,7 +882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380F055D-8AA9-42FE-BD6E-2FE0A974F2CE}">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -776,7 +932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C99316C-3880-404D-B909-A4EF9863EAAC}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>